<commit_message>
Mejoras en análisis, scripts de ejecución y documentación. Corrección de errores bivariados.
</commit_message>
<xml_diff>
--- a/resultados_analisis.xlsx
+++ b/resultados_analisis.xlsx
@@ -19,6 +19,20 @@
     <sheet name="PREGUNTA_4" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Personas_vs_Empresas_inferencia" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="WordFreq_PREGUNTA_5" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="CIUDAD_AGENCIA_vs_TIPO_EJECUTIVO" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="CIUDAD_AGENCIA_vs_SEGMENTO" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="TIPO_EJECUTIVO_vs_SEGMENTO" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="GENERO_vs_CIUDAD_AGENCIA" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="GENERO_vs_SEGMENTO" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="ESTRATO_vs_SEGMENTO" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="GENERO_vs_TIPO_EJECUTIVO" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="AGENCIA_EJECUTIVO_vs_SEGMENTO" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="CIUDAD_AGENCIA_vs_PREGUNTA_1" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="TIPO_EJECUTIVO_vs_PREGUNTA_1" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="SEGMENTO_vs_PREGUNTA_1" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="GENERO_vs_PREGUNTA_1" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="ESTRATO_vs_PREGUNTA_1" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="AGENCIA_EJECUTIVO_vs_PREGUNTA_1" sheetId="26" state="visible" r:id="rId26"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -996,6 +1010,730 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CIUDAD_AGENCIA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE AGENCIA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE CUENTA EMPRESAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bogota D.C.</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>95.6442831215971</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4.355716878402903</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>100</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>95.72368421052632</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4.276315789473684</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>100</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CIUDAD_AGENCIA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bogota D.C.</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4.355716878402903</v>
+      </c>
+      <c r="C3" t="n">
+        <v>95.6442831215971</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.276315789473684</v>
+      </c>
+      <c r="C7" t="n">
+        <v>95.72368421052632</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>TIPO_EJECUTIVO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE AGENCIA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE CUENTA EMPRESAS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Bogota D.C.</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.345058626465661</v>
+      </c>
+      <c r="C2" t="n">
+        <v>48.91122278056951</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6.365159128978225</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.010050251256281</v>
+      </c>
+      <c r="F2" t="n">
+        <v>8.040201005025125</v>
+      </c>
+      <c r="G2" t="n">
+        <v>30.82077051926298</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.507537688442211</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.864801864801865</v>
+      </c>
+      <c r="C3" t="n">
+        <v>54.77855477855478</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.428904428904429</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.729603729603729</v>
+      </c>
+      <c r="F3" t="n">
+        <v>8.391608391608392</v>
+      </c>
+      <c r="G3" t="n">
+        <v>24.94172494172494</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.864801864801865</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>64.86486486486487</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>35.13513513513514</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ESTRATO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>100</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE AGENCIA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE CUENTA EMPRESAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -1051,6 +1789,1735 @@
       </c>
       <c r="C3" t="n">
         <v>3.48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>AGENCIA_EJECUTIVO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Centro Internacional</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15.21739130434783</v>
+      </c>
+      <c r="C3" t="n">
+        <v>84.78260869565217</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Centro Mayor</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Bogota El Nogal</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Gran Estacion</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Plaza Imperial</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Principal</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>23.28767123287671</v>
+      </c>
+      <c r="C8" t="n">
+        <v>76.71232876712328</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Santa Fe</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Coltejer Principal</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>10.23622047244094</v>
+      </c>
+      <c r="C12" t="n">
+        <v>89.76377952755905</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>San Diego</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Unicentro</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CIUDAD_AGENCIA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Minimo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mediana</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maximo</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Desviacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>17</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4.882352941176471</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.3321055820775357</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>28</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4.642857142857143</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.8261595987094037</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>22</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4.590909090909091</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.7963662060880873</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>84</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.547619047619047</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.7976586506810486</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>57</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4.526315789473684</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.07080182169876</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>304</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.457236842105263</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.8353653356769846</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Bogota D.C.</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>551</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4.277676950998185</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.9839765578298537</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>TIPO_EJECUTIVO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Minimo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mediana</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maximo</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Desviacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE AGENCIA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1026</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4.409356725146199</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.9074596949666</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE CUENTA EMPRESAS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>37</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.837837837837838</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.258604021956105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SEGMENTO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Minimo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mediana</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maximo</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Desviacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1026</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4.409356725146199</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.9074596949666</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>37</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.837837837837838</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.258604021956105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Minimo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mediana</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maximo</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Desviacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>597</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4.445561139028475</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8969380585655836</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>429</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4.358974358974359</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9205823389566764</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>37</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.837837837837838</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.258604021956105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ESTRATO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Minimo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mediana</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maximo</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Desviacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" t="n">
+        <v>173</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4.468208092485549</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.9120483734514999</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>102</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4.431372549019608</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9493072400812425</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>298</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4.426174496644295</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9043029179584666</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>348</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.382183908045977</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.885635511950874</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>98</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4.336734693877551</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.9626411001250184</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.285714285714286</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.7559289460184544</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>37</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.837837837837838</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.258604021956105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>AGENCIA_EJECUTIVO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Minimo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mediana</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maximo</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Desviacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>17</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4.882352941176471</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.3321055820775357</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>28</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4.642857142857143</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.8261595987094037</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Santa Fe</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>57</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4.614035087719298</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.6749176130915187</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>22</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.590909090909091</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.7963662060880873</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>84</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4.547619047619047</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.7976586506810486</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>57</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.526315789473684</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.07080182169876</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Unicentro</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>119</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4.495798319327731</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.8524535832070713</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Coltejer Principal</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>127</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4.440944881889764</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>5</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.8512692979150622</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>San Diego</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.413793103448276</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>5</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.7731113434850687</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Gran Estacion</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>58</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4.396551724137931</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" t="n">
+        <v>5</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.7478543617580123</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Centro Internacional</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>46</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>5</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4.347826086956522</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5</v>
+      </c>
+      <c r="H12" t="n">
+        <v>5</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.8747670497362986</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Centro Mayor</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>73</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4.342465753424658</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5</v>
+      </c>
+      <c r="H13" t="n">
+        <v>5</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.8534110980548034</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Plaza Imperial</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>86</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4.313953488372093</v>
+      </c>
+      <c r="G14" t="n">
+        <v>5</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.9488274858008791</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Principal</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>73</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4.260273972602739</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5</v>
+      </c>
+      <c r="H15" t="n">
+        <v>5</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1.000380445134555</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Bogota El Nogal</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>158</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4.050632911392405</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1.193386597626275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Excel engine and JSON serialization
</commit_message>
<xml_diff>
--- a/resultados_analisis.xlsx
+++ b/resultados_analisis.xlsx
@@ -33,6 +33,22 @@
     <sheet name="GENERO_vs_PREGUNTA_1" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="ESTRATO_vs_PREGUNTA_1" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="AGENCIA_EJECUTIVO_vs_PREGUNTA_1" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="CIUDAD_AGENCIA_vs_TIPO_EJECUTIVO_abs" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="CIUDAD_AGENCIA_vs_TIPO_EJECUTIVO_pct" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="CIUDAD_AGENCIA_vs_SEGMENTO_abs" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="CIUDAD_AGENCIA_vs_SEGMENTO_pct" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="TIPO_EJECUTIVO_vs_SEGMENTO_abs" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="TIPO_EJECUTIVO_vs_SEGMENTO_pct" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="GENERO_vs_CIUDAD_AGENCIA_abs" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="GENERO_vs_CIUDAD_AGENCIA_pct" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="GENERO_vs_SEGMENTO_abs" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="GENERO_vs_SEGMENTO_pct" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="ESTRATO_vs_SEGMENTO_abs" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="ESTRATO_vs_SEGMENTO_pct" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="GENERO_vs_TIPO_EJECUTIVO_abs" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="GENERO_vs_TIPO_EJECUTIVO_pct" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="AGENCIA_EJECUTIVO_vs_SEGMENTO_abs" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="AGENCIA_EJECUTIVO_vs_SEGMENTO_pct" sheetId="42" state="visible" r:id="rId42"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2033,7 +2049,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2087,6 +2103,21 @@
           <t>Desviacion</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Error_estandar</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_inf</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_sup</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -2118,6 +2149,15 @@
       <c r="I2" t="n">
         <v>0.3321055820775357</v>
       </c>
+      <c r="J2" t="n">
+        <v>0.08054743492723031</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.711600007035576</v>
+      </c>
+      <c r="L2" t="n">
+        <v>5.053105875317366</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2149,6 +2189,15 @@
       <c r="I3" t="n">
         <v>0.8261595987094037</v>
       </c>
+      <c r="J3" t="n">
+        <v>0.1561294886738571</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4.32250589347366</v>
+      </c>
+      <c r="L3" t="n">
+        <v>4.963208392240626</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2180,6 +2229,15 @@
       <c r="I4" t="n">
         <v>0.7963662060880873</v>
       </c>
+      <c r="J4" t="n">
+        <v>0.16978584561938</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4.237820095720235</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4.943998086097947</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2211,6 +2269,15 @@
       <c r="I5" t="n">
         <v>0.7976586506810486</v>
       </c>
+      <c r="J5" t="n">
+        <v>0.08703169394005343</v>
+      </c>
+      <c r="K5" t="n">
+        <v>4.374516508771767</v>
+      </c>
+      <c r="L5" t="n">
+        <v>4.720721586466328</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -2242,6 +2309,15 @@
       <c r="I6" t="n">
         <v>1.07080182169876</v>
       </c>
+      <c r="J6" t="n">
+        <v>0.1418311660844202</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4.242193822371698</v>
+      </c>
+      <c r="L6" t="n">
+        <v>4.81043775657567</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2273,6 +2349,15 @@
       <c r="I7" t="n">
         <v>0.8353653356769846</v>
       </c>
+      <c r="J7" t="n">
+        <v>0.04791148788359088</v>
+      </c>
+      <c r="K7" t="n">
+        <v>4.36295546168879</v>
+      </c>
+      <c r="L7" t="n">
+        <v>4.551518222521736</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -2303,6 +2388,15 @@
       </c>
       <c r="I8" t="n">
         <v>0.9839765578298537</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0419188106976587</v>
+      </c>
+      <c r="K8" t="n">
+        <v>4.195336394914545</v>
+      </c>
+      <c r="L8" t="n">
+        <v>4.360017507081825</v>
       </c>
     </row>
   </sheetData>
@@ -2316,7 +2410,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2370,6 +2464,21 @@
           <t>Desviacion</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Error_estandar</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_inf</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_sup</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -2401,6 +2510,15 @@
       <c r="I2" t="n">
         <v>0.9074596949666</v>
       </c>
+      <c r="J2" t="n">
+        <v>0.02833046249626565</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.353764394478435</v>
+      </c>
+      <c r="L2" t="n">
+        <v>4.464949055813963</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2431,6 +2549,15 @@
       </c>
       <c r="I3" t="n">
         <v>1.258604021956105</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.2069132266280334</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3.418198364190015</v>
+      </c>
+      <c r="L3" t="n">
+        <v>4.25747731148566</v>
       </c>
     </row>
   </sheetData>
@@ -2444,7 +2571,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2498,6 +2625,21 @@
           <t>Desviacion</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Error_estandar</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_inf</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_sup</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -2529,6 +2671,15 @@
       <c r="I2" t="n">
         <v>0.9074596949666</v>
       </c>
+      <c r="J2" t="n">
+        <v>0.02833046249626565</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.353764394478435</v>
+      </c>
+      <c r="L2" t="n">
+        <v>4.464949055813963</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2559,6 +2710,15 @@
       </c>
       <c r="I3" t="n">
         <v>1.258604021956105</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.2069132266280334</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3.418198364190015</v>
+      </c>
+      <c r="L3" t="n">
+        <v>4.25747731148566</v>
       </c>
     </row>
   </sheetData>
@@ -2572,7 +2732,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2626,6 +2786,21 @@
           <t>Desviacion</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Error_estandar</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_inf</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_sup</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -2657,6 +2832,15 @@
       <c r="I2" t="n">
         <v>0.8969380585655836</v>
       </c>
+      <c r="J2" t="n">
+        <v>0.03670923098764376</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.373465961744565</v>
+      </c>
+      <c r="L2" t="n">
+        <v>4.517656316312386</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2688,6 +2872,15 @@
       <c r="I3" t="n">
         <v>0.9205823389566764</v>
       </c>
+      <c r="J3" t="n">
+        <v>0.04444613415161304</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4.271614499374247</v>
+      </c>
+      <c r="L3" t="n">
+        <v>4.44633421857447</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2718,6 +2911,15 @@
       </c>
       <c r="I4" t="n">
         <v>1.258604021956105</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.2069132266280334</v>
+      </c>
+      <c r="K4" t="n">
+        <v>3.418198364190015</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4.25747731148566</v>
       </c>
     </row>
   </sheetData>
@@ -2731,7 +2933,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2785,6 +2987,21 @@
           <t>Desviacion</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Error_estandar</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_inf</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_sup</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -2813,6 +3030,15 @@
       </c>
       <c r="I2" t="n">
         <v>0.9120483734514999</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.06934175378521099</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.331337721340395</v>
+      </c>
+      <c r="L2" t="n">
+        <v>4.605078463630703</v>
       </c>
     </row>
     <row r="3">
@@ -2843,6 +3069,15 @@
       <c r="I3" t="n">
         <v>0.9493072400812425</v>
       </c>
+      <c r="J3" t="n">
+        <v>0.09399542312964103</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4.244910914028019</v>
+      </c>
+      <c r="L3" t="n">
+        <v>4.617834184011198</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -2872,6 +3107,15 @@
       <c r="I4" t="n">
         <v>0.9043029179584666</v>
       </c>
+      <c r="J4" t="n">
+        <v>0.05238486151744608</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4.323081952198863</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4.529267041089727</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -2901,6 +3145,15 @@
       <c r="I5" t="n">
         <v>0.885635511950874</v>
       </c>
+      <c r="J5" t="n">
+        <v>0.047475046683001</v>
+      </c>
+      <c r="K5" t="n">
+        <v>4.288808846673866</v>
+      </c>
+      <c r="L5" t="n">
+        <v>4.475558969418088</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -2930,6 +3183,15 @@
       <c r="I6" t="n">
         <v>0.9626411001250184</v>
       </c>
+      <c r="J6" t="n">
+        <v>0.09724143567818269</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4.143737361844497</v>
+      </c>
+      <c r="L6" t="n">
+        <v>4.529732025910604</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -2959,6 +3221,15 @@
       <c r="I7" t="n">
         <v>0.7559289460184544</v>
       </c>
+      <c r="J7" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K7" t="n">
+        <v>3.58659661395858</v>
+      </c>
+      <c r="L7" t="n">
+        <v>4.984831957469991</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -2987,6 +3258,15 @@
       </c>
       <c r="I8" t="n">
         <v>1.258604021956105</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.2069132266280334</v>
+      </c>
+      <c r="K8" t="n">
+        <v>3.418198364190015</v>
+      </c>
+      <c r="L8" t="n">
+        <v>4.25747731148566</v>
       </c>
     </row>
   </sheetData>
@@ -3000,7 +3280,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3054,6 +3334,21 @@
           <t>Desviacion</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Error_estandar</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_inf</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>IC_95_sup</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -3085,6 +3380,15 @@
       <c r="I2" t="n">
         <v>0.3321055820775357</v>
       </c>
+      <c r="J2" t="n">
+        <v>0.08054743492723031</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.711600007035576</v>
+      </c>
+      <c r="L2" t="n">
+        <v>5.053105875317366</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -3116,6 +3420,15 @@
       <c r="I3" t="n">
         <v>0.8261595987094037</v>
       </c>
+      <c r="J3" t="n">
+        <v>0.1561294886738571</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4.32250589347366</v>
+      </c>
+      <c r="L3" t="n">
+        <v>4.963208392240626</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -3147,6 +3460,15 @@
       <c r="I4" t="n">
         <v>0.6749176130915187</v>
       </c>
+      <c r="J4" t="n">
+        <v>0.08939502168928225</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4.434955340209039</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4.793114835229557</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -3178,6 +3500,15 @@
       <c r="I5" t="n">
         <v>0.7963662060880873</v>
       </c>
+      <c r="J5" t="n">
+        <v>0.16978584561938</v>
+      </c>
+      <c r="K5" t="n">
+        <v>4.237820095720235</v>
+      </c>
+      <c r="L5" t="n">
+        <v>4.943998086097947</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -3209,6 +3540,15 @@
       <c r="I6" t="n">
         <v>0.7976586506810486</v>
       </c>
+      <c r="J6" t="n">
+        <v>0.08703169394005343</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4.374516508771767</v>
+      </c>
+      <c r="L6" t="n">
+        <v>4.720721586466328</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -3240,6 +3580,15 @@
       <c r="I7" t="n">
         <v>1.07080182169876</v>
       </c>
+      <c r="J7" t="n">
+        <v>0.1418311660844202</v>
+      </c>
+      <c r="K7" t="n">
+        <v>4.242193822371698</v>
+      </c>
+      <c r="L7" t="n">
+        <v>4.81043775657567</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -3271,6 +3620,15 @@
       <c r="I8" t="n">
         <v>0.8524535832070713</v>
       </c>
+      <c r="J8" t="n">
+        <v>0.07814429185122354</v>
+      </c>
+      <c r="K8" t="n">
+        <v>4.341051346738187</v>
+      </c>
+      <c r="L8" t="n">
+        <v>4.650545291917275</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -3302,6 +3660,15 @@
       <c r="I9" t="n">
         <v>0.8512692979150622</v>
       </c>
+      <c r="J9" t="n">
+        <v>0.07553793527710158</v>
+      </c>
+      <c r="K9" t="n">
+        <v>4.291457528643064</v>
+      </c>
+      <c r="L9" t="n">
+        <v>4.590432235136464</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -3333,6 +3700,15 @@
       <c r="I10" t="n">
         <v>0.7731113434850687</v>
       </c>
+      <c r="J10" t="n">
+        <v>0.101514492716412</v>
+      </c>
+      <c r="K10" t="n">
+        <v>4.210513838166213</v>
+      </c>
+      <c r="L10" t="n">
+        <v>4.617072368730339</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -3364,6 +3740,15 @@
       <c r="I11" t="n">
         <v>0.7478543617580123</v>
       </c>
+      <c r="J11" t="n">
+        <v>0.0981980885410291</v>
+      </c>
+      <c r="K11" t="n">
+        <v>4.199913443666119</v>
+      </c>
+      <c r="L11" t="n">
+        <v>4.593190004609742</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -3395,6 +3780,15 @@
       <c r="I12" t="n">
         <v>0.8747670497362986</v>
       </c>
+      <c r="J12" t="n">
+        <v>0.1289773649929681</v>
+      </c>
+      <c r="K12" t="n">
+        <v>4.088052339035262</v>
+      </c>
+      <c r="L12" t="n">
+        <v>4.607599834877781</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -3426,6 +3820,15 @@
       <c r="I13" t="n">
         <v>0.8534110980548034</v>
       </c>
+      <c r="J13" t="n">
+        <v>0.09988421394624364</v>
+      </c>
+      <c r="K13" t="n">
+        <v>4.143350212038161</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4.541581294811154</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -3457,6 +3860,15 @@
       <c r="I14" t="n">
         <v>0.9488274858008791</v>
       </c>
+      <c r="J14" t="n">
+        <v>0.1023146990855549</v>
+      </c>
+      <c r="K14" t="n">
+        <v>4.110524455717095</v>
+      </c>
+      <c r="L14" t="n">
+        <v>4.51738252102709</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -3488,6 +3900,15 @@
       <c r="I15" t="n">
         <v>1.000380445134555</v>
       </c>
+      <c r="J15" t="n">
+        <v>0.1170856749311241</v>
+      </c>
+      <c r="K15" t="n">
+        <v>4.026867945449529</v>
+      </c>
+      <c r="L15" t="n">
+        <v>4.49367999975595</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -3518,6 +3939,396 @@
       </c>
       <c r="I16" t="n">
         <v>1.193386597626275</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.09494074005792742</v>
+      </c>
+      <c r="K16" t="n">
+        <v>3.863106990496249</v>
+      </c>
+      <c r="L16" t="n">
+        <v>4.238158832288562</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CIUDAD_AGENCIA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE AGENCIA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE CUENTA EMPRESAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>22</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bogota D.C.</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>527</v>
+      </c>
+      <c r="C3" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>57</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>28</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>84</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>291</v>
+      </c>
+      <c r="C7" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>17</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CIUDAD_AGENCIA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE AGENCIA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE CUENTA EMPRESAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bogota D.C.</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>95.6442831215971</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4.355716878402903</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>100</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>95.72368421052632</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4.276315789473684</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>100</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CIUDAD_AGENCIA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bogota D.C.</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>24</v>
+      </c>
+      <c r="C3" t="n">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>13</v>
+      </c>
+      <c r="C7" t="n">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3587,6 +4398,998 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CIUDAD_AGENCIA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bogota D.C.</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4.355716878402903</v>
+      </c>
+      <c r="C3" t="n">
+        <v>95.6442831215971</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.276315789473684</v>
+      </c>
+      <c r="C7" t="n">
+        <v>95.72368421052632</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>TIPO_EJECUTIVO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE AGENCIA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE CUENTA EMPRESAS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>37</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>TIPO_EJECUTIVO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE AGENCIA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE CUENTA EMPRESAS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Bogota D.C.</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>14</v>
+      </c>
+      <c r="C2" t="n">
+        <v>292</v>
+      </c>
+      <c r="D2" t="n">
+        <v>38</v>
+      </c>
+      <c r="E2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F2" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2" t="n">
+        <v>184</v>
+      </c>
+      <c r="H2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>235</v>
+      </c>
+      <c r="D3" t="n">
+        <v>19</v>
+      </c>
+      <c r="E3" t="n">
+        <v>16</v>
+      </c>
+      <c r="F3" t="n">
+        <v>36</v>
+      </c>
+      <c r="G3" t="n">
+        <v>107</v>
+      </c>
+      <c r="H3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>13</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Bogota D.C.</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Medellin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.345058626465661</v>
+      </c>
+      <c r="C2" t="n">
+        <v>48.91122278056951</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6.365159128978225</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.010050251256281</v>
+      </c>
+      <c r="F2" t="n">
+        <v>8.040201005025125</v>
+      </c>
+      <c r="G2" t="n">
+        <v>30.82077051926298</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.507537688442211</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.864801864801865</v>
+      </c>
+      <c r="C3" t="n">
+        <v>54.77855477855478</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.428904428904429</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.729603729603729</v>
+      </c>
+      <c r="F3" t="n">
+        <v>8.391608391608392</v>
+      </c>
+      <c r="G3" t="n">
+        <v>24.94172494172494</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.864801864801865</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>64.86486486486487</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>35.13513513513514</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>37</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ESTRATO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>37</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ESTRATO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>100</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE AGENCIA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE CUENTA EMPRESAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>597</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>429</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -3655,6 +5458,543 @@
       </c>
       <c r="C4" t="n">
         <v>3.48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE AGENCIA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>GERENTE DE CUENTA EMPRESAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>AGENCIA_EJECUTIVO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Centro Internacional</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Centro Mayor</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Bogota El Nogal</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Gran Estacion</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Plaza Imperial</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Principal</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>17</v>
+      </c>
+      <c r="C8" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Santa Fe</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Coltejer Principal</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>13</v>
+      </c>
+      <c r="C12" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>San Diego</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Unicentro</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>AGENCIA_EJECUTIVO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Empresas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Personas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Centro Internacional</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15.21739130434783</v>
+      </c>
+      <c r="C3" t="n">
+        <v>84.78260869565217</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Centro Mayor</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Bogota El Nogal</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Gran Estacion</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Plaza Imperial</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Principal</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>23.28767123287671</v>
+      </c>
+      <c r="C8" t="n">
+        <v>76.71232876712328</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Bogota Santa Fe</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Bucaramanga</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Cali Norte</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Coltejer Principal</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>10.23622047244094</v>
+      </c>
+      <c r="C12" t="n">
+        <v>89.76377952755905</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Manizales</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>San Diego</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Unicentro</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>